<commit_message>
Pushing changed database schema and modified template
</commit_message>
<xml_diff>
--- a/excelFiles/smis__template.xlsx
+++ b/excelFiles/smis__template.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="40">
   <si>
     <t>MTWARA ISLAMIC SECONDARY SCHOOL</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>Amir</t>
+  </si>
+  <si>
+    <t>YEAR</t>
   </si>
 </sst>
 </file>
@@ -531,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M576"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11:K50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -735,6 +738,9 @@
       <c r="J10" s="4" t="s">
         <v>15</v>
       </c>
+      <c r="K10" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
@@ -767,6 +773,9 @@
       <c r="J11">
         <v>1</v>
       </c>
+      <c r="K11">
+        <v>2015</v>
+      </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
@@ -799,6 +808,9 @@
       <c r="J12">
         <v>1</v>
       </c>
+      <c r="K12">
+        <v>2015</v>
+      </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
@@ -831,6 +843,9 @@
       <c r="J13">
         <v>1</v>
       </c>
+      <c r="K13">
+        <v>2015</v>
+      </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
@@ -863,6 +878,9 @@
       <c r="J14">
         <v>1</v>
       </c>
+      <c r="K14">
+        <v>2015</v>
+      </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
@@ -895,152 +913,1275 @@
       <c r="J15">
         <v>1</v>
       </c>
+      <c r="K15">
+        <v>2015</v>
+      </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="H16" s="8"/>
-    </row>
-    <row r="17" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H17" s="8"/>
-    </row>
-    <row r="18" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H18" s="8"/>
-    </row>
-    <row r="19" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H19" s="8"/>
-    </row>
-    <row r="20" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H20" s="8"/>
-    </row>
-    <row r="21" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H21" s="8"/>
-    </row>
-    <row r="22" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H22" s="8"/>
-    </row>
-    <row r="23" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H23" s="8"/>
-    </row>
-    <row r="24" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H24" s="8"/>
-    </row>
-    <row r="25" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H25" s="8"/>
-    </row>
-    <row r="26" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H26" s="8"/>
-    </row>
-    <row r="27" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H27" s="8"/>
-    </row>
-    <row r="28" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H28" s="8"/>
-    </row>
-    <row r="29" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H29" s="8"/>
-    </row>
-    <row r="30" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H30" s="8"/>
-    </row>
-    <row r="31" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H31" s="8"/>
-    </row>
-    <row r="32" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H32" s="8"/>
-    </row>
-    <row r="33" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H33" s="8"/>
-    </row>
-    <row r="34" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H34" s="8"/>
-    </row>
-    <row r="35" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H35" s="8"/>
-    </row>
-    <row r="36" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H36" s="8"/>
-    </row>
-    <row r="37" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H37" s="8"/>
-    </row>
-    <row r="38" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H38" s="8"/>
-    </row>
-    <row r="39" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H39" s="8"/>
-    </row>
-    <row r="40" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H40" s="8"/>
-    </row>
-    <row r="41" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H41" s="8"/>
-    </row>
-    <row r="42" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H42" s="8"/>
-    </row>
-    <row r="43" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H43" s="8"/>
-    </row>
-    <row r="44" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H44" s="8"/>
-    </row>
-    <row r="45" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H45" s="8"/>
-    </row>
-    <row r="46" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H46" s="8"/>
-    </row>
-    <row r="47" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H47" s="8"/>
-    </row>
-    <row r="48" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H48" s="8"/>
-    </row>
-    <row r="49" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H49" s="8"/>
-    </row>
-    <row r="50" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H50" s="8"/>
-    </row>
-    <row r="51" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16" s="7">
+        <v>31506</v>
+      </c>
+      <c r="G16" t="s">
+        <v>23</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="I16" t="s">
+        <v>25</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="K16">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17" s="7">
+        <v>31507</v>
+      </c>
+      <c r="G17" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I17" t="s">
+        <v>25</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="K17">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18" s="7">
+        <v>31508</v>
+      </c>
+      <c r="G18" t="s">
+        <v>23</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I18" t="s">
+        <v>25</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+      <c r="K18">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19" s="7">
+        <v>31509</v>
+      </c>
+      <c r="G19" t="s">
+        <v>23</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I19" t="s">
+        <v>25</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
+      <c r="K19">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20" s="7">
+        <v>31510</v>
+      </c>
+      <c r="G20" t="s">
+        <v>23</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I20" t="s">
+        <v>25</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="K20">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21" s="7">
+        <v>31506</v>
+      </c>
+      <c r="G21" t="s">
+        <v>23</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="I21" t="s">
+        <v>25</v>
+      </c>
+      <c r="J21">
+        <v>1</v>
+      </c>
+      <c r="K21">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>2</v>
+      </c>
+      <c r="F22" s="7">
+        <v>31507</v>
+      </c>
+      <c r="G22" t="s">
+        <v>23</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I22" t="s">
+        <v>25</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+      <c r="K22">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23" s="7">
+        <v>31508</v>
+      </c>
+      <c r="G23" t="s">
+        <v>23</v>
+      </c>
+      <c r="H23" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I23" t="s">
+        <v>25</v>
+      </c>
+      <c r="J23">
+        <v>1</v>
+      </c>
+      <c r="K23">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24" s="7">
+        <v>31509</v>
+      </c>
+      <c r="G24" t="s">
+        <v>23</v>
+      </c>
+      <c r="H24" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I24" t="s">
+        <v>25</v>
+      </c>
+      <c r="J24">
+        <v>1</v>
+      </c>
+      <c r="K24">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25" s="7">
+        <v>31510</v>
+      </c>
+      <c r="G25" t="s">
+        <v>23</v>
+      </c>
+      <c r="H25" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I25" t="s">
+        <v>25</v>
+      </c>
+      <c r="J25">
+        <v>1</v>
+      </c>
+      <c r="K25">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26" s="7">
+        <v>31506</v>
+      </c>
+      <c r="G26" t="s">
+        <v>23</v>
+      </c>
+      <c r="H26" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="I26" t="s">
+        <v>25</v>
+      </c>
+      <c r="J26">
+        <v>1</v>
+      </c>
+      <c r="K26">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>2</v>
+      </c>
+      <c r="F27" s="7">
+        <v>31507</v>
+      </c>
+      <c r="G27" t="s">
+        <v>23</v>
+      </c>
+      <c r="H27" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I27" t="s">
+        <v>25</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
+      <c r="K27">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28" t="s">
+        <v>20</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28" s="7">
+        <v>31508</v>
+      </c>
+      <c r="G28" t="s">
+        <v>23</v>
+      </c>
+      <c r="H28" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I28" t="s">
+        <v>25</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
+      <c r="K28">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" t="s">
+        <v>20</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29" s="7">
+        <v>31509</v>
+      </c>
+      <c r="G29" t="s">
+        <v>23</v>
+      </c>
+      <c r="H29" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I29" t="s">
+        <v>25</v>
+      </c>
+      <c r="J29">
+        <v>1</v>
+      </c>
+      <c r="K29">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" t="s">
+        <v>38</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30" s="7">
+        <v>31510</v>
+      </c>
+      <c r="G30" t="s">
+        <v>23</v>
+      </c>
+      <c r="H30" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I30" t="s">
+        <v>25</v>
+      </c>
+      <c r="J30">
+        <v>1</v>
+      </c>
+      <c r="K30">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" t="s">
+        <v>20</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31" s="7">
+        <v>31506</v>
+      </c>
+      <c r="G31" t="s">
+        <v>23</v>
+      </c>
+      <c r="H31" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="I31" t="s">
+        <v>25</v>
+      </c>
+      <c r="J31">
+        <v>1</v>
+      </c>
+      <c r="K31">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>31</v>
+      </c>
+      <c r="C32" t="s">
+        <v>32</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>2</v>
+      </c>
+      <c r="F32" s="7">
+        <v>31507</v>
+      </c>
+      <c r="G32" t="s">
+        <v>23</v>
+      </c>
+      <c r="H32" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I32" t="s">
+        <v>25</v>
+      </c>
+      <c r="J32">
+        <v>1</v>
+      </c>
+      <c r="K32">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" t="s">
+        <v>20</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33" s="7">
+        <v>31508</v>
+      </c>
+      <c r="G33" t="s">
+        <v>23</v>
+      </c>
+      <c r="H33" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I33" t="s">
+        <v>25</v>
+      </c>
+      <c r="J33">
+        <v>1</v>
+      </c>
+      <c r="K33">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A34" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" t="s">
+        <v>20</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34" s="7">
+        <v>31509</v>
+      </c>
+      <c r="G34" t="s">
+        <v>23</v>
+      </c>
+      <c r="H34" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I34" t="s">
+        <v>25</v>
+      </c>
+      <c r="J34">
+        <v>1</v>
+      </c>
+      <c r="K34">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A35" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" t="s">
+        <v>37</v>
+      </c>
+      <c r="C35" t="s">
+        <v>38</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35" s="7">
+        <v>31510</v>
+      </c>
+      <c r="G35" t="s">
+        <v>23</v>
+      </c>
+      <c r="H35" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I35" t="s">
+        <v>25</v>
+      </c>
+      <c r="J35">
+        <v>1</v>
+      </c>
+      <c r="K35">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A36" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B36" t="s">
+        <v>19</v>
+      </c>
+      <c r="C36" t="s">
+        <v>20</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36" s="7">
+        <v>31506</v>
+      </c>
+      <c r="G36" t="s">
+        <v>23</v>
+      </c>
+      <c r="H36" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="I36" t="s">
+        <v>25</v>
+      </c>
+      <c r="J36">
+        <v>1</v>
+      </c>
+      <c r="K36">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A37" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B37" t="s">
+        <v>31</v>
+      </c>
+      <c r="C37" t="s">
+        <v>32</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <v>2</v>
+      </c>
+      <c r="F37" s="7">
+        <v>31507</v>
+      </c>
+      <c r="G37" t="s">
+        <v>23</v>
+      </c>
+      <c r="H37" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I37" t="s">
+        <v>25</v>
+      </c>
+      <c r="J37">
+        <v>1</v>
+      </c>
+      <c r="K37">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A38" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B38" t="s">
+        <v>34</v>
+      </c>
+      <c r="C38" t="s">
+        <v>20</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38" s="7">
+        <v>31508</v>
+      </c>
+      <c r="G38" t="s">
+        <v>23</v>
+      </c>
+      <c r="H38" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I38" t="s">
+        <v>25</v>
+      </c>
+      <c r="J38">
+        <v>1</v>
+      </c>
+      <c r="K38">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A39" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B39" t="s">
+        <v>34</v>
+      </c>
+      <c r="C39" t="s">
+        <v>20</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39" s="7">
+        <v>31509</v>
+      </c>
+      <c r="G39" t="s">
+        <v>23</v>
+      </c>
+      <c r="H39" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I39" t="s">
+        <v>25</v>
+      </c>
+      <c r="J39">
+        <v>1</v>
+      </c>
+      <c r="K39">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A40" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B40" t="s">
+        <v>37</v>
+      </c>
+      <c r="C40" t="s">
+        <v>38</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40" s="7">
+        <v>31510</v>
+      </c>
+      <c r="G40" t="s">
+        <v>23</v>
+      </c>
+      <c r="H40" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I40" t="s">
+        <v>25</v>
+      </c>
+      <c r="J40">
+        <v>1</v>
+      </c>
+      <c r="K40">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A41" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B41" t="s">
+        <v>19</v>
+      </c>
+      <c r="C41" t="s">
+        <v>20</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="F41" s="7">
+        <v>31506</v>
+      </c>
+      <c r="G41" t="s">
+        <v>23</v>
+      </c>
+      <c r="H41" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="I41" t="s">
+        <v>25</v>
+      </c>
+      <c r="J41">
+        <v>1</v>
+      </c>
+      <c r="K41">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A42" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B42" t="s">
+        <v>31</v>
+      </c>
+      <c r="C42" t="s">
+        <v>32</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>2</v>
+      </c>
+      <c r="F42" s="7">
+        <v>31507</v>
+      </c>
+      <c r="G42" t="s">
+        <v>23</v>
+      </c>
+      <c r="H42" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I42" t="s">
+        <v>25</v>
+      </c>
+      <c r="J42">
+        <v>1</v>
+      </c>
+      <c r="K42">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A43" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B43" t="s">
+        <v>34</v>
+      </c>
+      <c r="C43" t="s">
+        <v>20</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+      <c r="F43" s="7">
+        <v>31508</v>
+      </c>
+      <c r="G43" t="s">
+        <v>23</v>
+      </c>
+      <c r="H43" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I43" t="s">
+        <v>25</v>
+      </c>
+      <c r="J43">
+        <v>1</v>
+      </c>
+      <c r="K43">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A44" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B44" t="s">
+        <v>34</v>
+      </c>
+      <c r="C44" t="s">
+        <v>20</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <v>1</v>
+      </c>
+      <c r="F44" s="7">
+        <v>31509</v>
+      </c>
+      <c r="G44" t="s">
+        <v>23</v>
+      </c>
+      <c r="H44" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I44" t="s">
+        <v>25</v>
+      </c>
+      <c r="J44">
+        <v>1</v>
+      </c>
+      <c r="K44">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A45" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B45" t="s">
+        <v>37</v>
+      </c>
+      <c r="C45" t="s">
+        <v>38</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
+      <c r="F45" s="7">
+        <v>31510</v>
+      </c>
+      <c r="G45" t="s">
+        <v>23</v>
+      </c>
+      <c r="H45" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I45" t="s">
+        <v>25</v>
+      </c>
+      <c r="J45">
+        <v>1</v>
+      </c>
+      <c r="K45">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A46" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B46" t="s">
+        <v>19</v>
+      </c>
+      <c r="C46" t="s">
+        <v>20</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>1</v>
+      </c>
+      <c r="F46" s="7">
+        <v>31506</v>
+      </c>
+      <c r="G46" t="s">
+        <v>23</v>
+      </c>
+      <c r="H46" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="I46" t="s">
+        <v>25</v>
+      </c>
+      <c r="J46">
+        <v>1</v>
+      </c>
+      <c r="K46">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A47" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B47" t="s">
+        <v>31</v>
+      </c>
+      <c r="C47" t="s">
+        <v>32</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <v>2</v>
+      </c>
+      <c r="F47" s="7">
+        <v>31507</v>
+      </c>
+      <c r="G47" t="s">
+        <v>23</v>
+      </c>
+      <c r="H47" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I47" t="s">
+        <v>25</v>
+      </c>
+      <c r="J47">
+        <v>1</v>
+      </c>
+      <c r="K47">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A48" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B48" t="s">
+        <v>34</v>
+      </c>
+      <c r="C48" t="s">
+        <v>20</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="F48" s="7">
+        <v>31508</v>
+      </c>
+      <c r="G48" t="s">
+        <v>23</v>
+      </c>
+      <c r="H48" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I48" t="s">
+        <v>25</v>
+      </c>
+      <c r="J48">
+        <v>1</v>
+      </c>
+      <c r="K48">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A49" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B49" t="s">
+        <v>34</v>
+      </c>
+      <c r="C49" t="s">
+        <v>20</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
+      <c r="F49" s="7">
+        <v>31509</v>
+      </c>
+      <c r="G49" t="s">
+        <v>23</v>
+      </c>
+      <c r="H49" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I49" t="s">
+        <v>25</v>
+      </c>
+      <c r="J49">
+        <v>1</v>
+      </c>
+      <c r="K49">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A50" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B50" t="s">
+        <v>37</v>
+      </c>
+      <c r="C50" t="s">
+        <v>38</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="F50" s="7">
+        <v>31510</v>
+      </c>
+      <c r="G50" t="s">
+        <v>23</v>
+      </c>
+      <c r="H50" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I50" t="s">
+        <v>25</v>
+      </c>
+      <c r="J50">
+        <v>1</v>
+      </c>
+      <c r="K50">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="H51" s="8"/>
     </row>
-    <row r="52" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="H52" s="8"/>
     </row>
-    <row r="53" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="H53" s="8"/>
     </row>
-    <row r="54" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="H54" s="8"/>
     </row>
-    <row r="55" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="H55" s="8"/>
     </row>
-    <row r="56" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="H56" s="8"/>
     </row>
-    <row r="57" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="H57" s="8"/>
     </row>
-    <row r="58" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="H58" s="8"/>
     </row>
-    <row r="59" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="H59" s="8"/>
     </row>
-    <row r="60" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="H60" s="8"/>
     </row>
-    <row r="61" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="H61" s="8"/>
     </row>
-    <row r="62" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="H62" s="8"/>
     </row>
-    <row r="63" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="H63" s="8"/>
     </row>
-    <row r="64" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="H64" s="8"/>
     </row>
     <row r="65" spans="8:8" x14ac:dyDescent="0.3">

</xml_diff>